<commit_message>
set max cap by source - geothermal 1,000 MWs
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\eps-mexico\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824FA9A3-A4E7-4476-991D-02FD2428D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="405" windowWidth="22755" windowHeight="12300"/>
+    <workbookView xWindow="2140" yWindow="1120" windowWidth="21120" windowHeight="12490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="MPCbS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -299,7 +311,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
@@ -523,6 +535,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -558,6 +587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -733,24 +779,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,120 +804,120 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B21" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -879,26 +925,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
     <col min="4" max="4" width="71" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -915,7 +961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -932,7 +978,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -949,7 +995,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -966,7 +1012,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -983,7 +1029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1000,7 +1046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1055,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1070,7 @@
         <v>187.60000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1033,7 +1079,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1042,7 +1088,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1053,12 +1099,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>32</v>
       </c>
@@ -1066,12 +1112,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -1094,7 +1140,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>56</v>
       </c>
@@ -1106,7 +1152,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>33</v>
       </c>
@@ -1122,7 +1168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1186,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -1149,7 +1195,7 @@
         <v>62000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
@@ -1161,7 +1207,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>57</v>
       </c>
@@ -1179,7 +1225,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D24" s="18" t="s">
         <v>69</v>
       </c>
@@ -1190,7 +1236,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>62</v>
       </c>
@@ -1204,7 +1250,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>63</v>
       </c>
@@ -1218,7 +1264,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>64</v>
       </c>
@@ -1232,12 +1278,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>73</v>
       </c>
@@ -1248,27 +1294,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D30" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>78</v>
       </c>
@@ -1277,7 +1323,7 @@
         <v>3.4127613941018762</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>80</v>
       </c>
@@ -1295,21 +1341,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -1317,7 +1365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1326,7 +1374,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1335,7 +1383,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1344,7 +1392,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1401,7 @@
         <v>187600.00000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1362,7 +1410,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1419,7 @@
         <v>154864000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1380,7 +1428,7 @@
         <v>38000000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1389,16 +1437,15 @@
         <v>62000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>40</v>
       </c>
       <c r="B10">
-        <f>Data!B22</f>
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1407,7 +1454,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1416,7 +1463,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1425,7 +1472,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1434,7 +1481,7 @@
         <v>4200000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1443,7 +1490,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1452,7 +1499,7 @@
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Use Mexico data for max potential capacity by source
</commit_message>
<xml_diff>
--- a/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
+++ b/InputData/elec/MPCbS/Max Potential Capacity by Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\eps-mexico\InputData\elec\MPCbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\Mexico\Models\eps-mexico\InputData\elec\MPCbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824FA9A3-A4E7-4476-991D-02FD2428D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CE6D66-0C19-438F-82F6-819D559316FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1120" windowWidth="21120" windowHeight="12490" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,62 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>Solar, Wind, Biomass</t>
-  </si>
-  <si>
-    <t>Hydropower</t>
-  </si>
-  <si>
     <t>National Renewable Energy Laboratory</t>
   </si>
   <si>
-    <t>U.S. Renewable Energy Technical Potentials: A GIS-Based Analysis</t>
-  </si>
-  <si>
-    <t>http://www.nrel.gov/docs/fy12osti/51946.pdf</t>
-  </si>
-  <si>
-    <t>Page iv, Table ES-1</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Potential Capacity (GW)</t>
-  </si>
-  <si>
-    <t>Urban utility-scale PV</t>
-  </si>
-  <si>
-    <t>Rural utility-scale PV</t>
-  </si>
-  <si>
-    <t>Concentrating Solar</t>
-  </si>
-  <si>
-    <t>Onshore wind</t>
-  </si>
-  <si>
-    <t>Offshore wind</t>
-  </si>
-  <si>
-    <t>Biopower</t>
-  </si>
-  <si>
-    <t>Hydrothermal power systems</t>
-  </si>
-  <si>
-    <t>Enhanced geothermal systems</t>
-  </si>
-  <si>
-    <t>Rooftop PV</t>
-  </si>
-  <si>
     <t>The max potential hydropower estimate here is substantially lower than</t>
   </si>
   <si>
@@ -128,12 +80,6 @@
     <t>hydropower potential (above).</t>
   </si>
   <si>
-    <t>Table ES-1 from NREL</t>
-  </si>
-  <si>
-    <t>Red = not used in model</t>
-  </si>
-  <si>
     <t>solar PV</t>
   </si>
   <si>
@@ -185,18 +131,6 @@
     <t>See Figure O3-8</t>
   </si>
   <si>
-    <t>Figures O3-3 and O3-8</t>
-  </si>
-  <si>
-    <t>https://energy.gov/sites/prod/files/2016/10/f33/Hydropower-Vision-Chapter-3-10212016.pdf</t>
-  </si>
-  <si>
-    <t>US Department of Energy</t>
-  </si>
-  <si>
-    <t>Chapter 3: Assessment of National Hydropower Potential</t>
-  </si>
-  <si>
     <t>lignite</t>
   </si>
   <si>
@@ -306,6 +240,27 @@
   </si>
   <si>
     <t>this limit doesn't come into play for these three electricity sources.)</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy22osti/82580.pdf</t>
+  </si>
+  <si>
+    <t>Mexico Clean Energy Report - Executive Summary</t>
+  </si>
+  <si>
+    <t>Solar, Onshore Wind, Geothermal, Hydro</t>
+  </si>
+  <si>
+    <t>Offshore Wind</t>
+  </si>
+  <si>
+    <t>ESMAP</t>
+  </si>
+  <si>
+    <t>https://documents1.worldbank.org/curated/en/540571586840981675/pdf/Technical-Potential-for-Offshore-Wind-in-Mexico-Map.pdf</t>
+  </si>
+  <si>
+    <t>Offshore Wind Technical Potential in Mexico</t>
   </si>
 </sst>
 </file>
@@ -363,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,12 +328,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +352,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -413,13 +362,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -439,7 +384,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -783,560 +728,470 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.81640625" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B14" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="4">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B23" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="71" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9">
+        <f>1.2*1000</f>
+        <v>1200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>101.2</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1200</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="8">
-        <v>101.2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>153000</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="9">
+        <f>3669*1000</f>
+        <v>3669000</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="8">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7">
         <v>6.9</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>664</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9">
+        <f>24918*1000</f>
+        <v>24918000</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="15">
-        <v>38000</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9">
+        <f>(8310+4105+516)*1000</f>
+        <v>12931000</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>11000</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9">
+        <f>B8</f>
+        <v>2500</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6">
         <v>65.5</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="15">
-        <v>4200</v>
-      </c>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>62</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="9">
+        <f>2.5*1000</f>
+        <v>2500</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="9">
+        <f>869*1000</f>
+        <v>869000</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8">
         <f>SUM(E3:E7)</f>
         <v>187.60000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="10">
-        <v>38</v>
-      </c>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="15">
-        <v>4000</v>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="10">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="11">
-        <f>E9*1000</f>
-        <v>187600.00000000003</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1820</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="21">
+        <v>262.39999999999998</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="17">
+        <v>33.57</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="19">
+        <v>67.8</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="19">
+        <v>23.4</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="19">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="22">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="11">
-        <f>B7*1000</f>
-        <v>11000000</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="11">
-        <f>SUM(B3:B5)*1000</f>
-        <v>154864000</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="11">
-        <f>B6*1000</f>
-        <v>38000000</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="20">
-        <v>1820</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="11">
-        <f>B9*1000</f>
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="11">
-        <f>B11*1000</f>
-        <v>4000000</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="11">
-        <f>B8*1000</f>
-        <v>4200000</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="23">
-        <v>262.39999999999998</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D24" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="19">
-        <v>33.57</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="21">
-        <v>67.8</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="21">
-        <v>23.4</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="21">
-        <v>137.69999999999999</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="24">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D30" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="26">
+      <c r="E36" s="24">
         <f>E27*E29/E24</f>
         <v>3.4127613941018762</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="27">
+        <v>58</v>
+      </c>
+      <c r="E37" s="25">
         <f>E20*(1+E36)</f>
         <v>8031.2257372654149</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B19" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1348,162 +1203,162 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="16">
+        <v>33</v>
+      </c>
+      <c r="B2" s="14">
         <f>9*10^12</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="16">
+        <v>21</v>
+      </c>
+      <c r="B3" s="14">
         <f>9*10^12</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="16">
+        <v>18</v>
+      </c>
+      <c r="B4" s="14">
         <f>9*10^12</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <f>Data!B17</f>
-        <v>187600.00000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B3</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B6">
-        <f>Data!B18</f>
-        <v>11000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B4</f>
+        <v>3669000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <f>Data!B19</f>
-        <v>154864000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B5</f>
+        <v>24918000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <f>Data!B20</f>
-        <v>38000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B6</f>
+        <v>12931000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <f>Data!B21</f>
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B7</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="16">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14">
         <f>9*10^12</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="16">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14">
         <f>9*10^12</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="16">
+        <v>32</v>
+      </c>
+      <c r="B13" s="14">
         <f>B2</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <f>Data!B23</f>
-        <v>4200000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <f>Data!B9</f>
+        <v>869000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="16">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14">
         <f>B11</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="16">
+        <v>37</v>
+      </c>
+      <c r="B16" s="14">
         <f>B11</f>
         <v>9000000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="16">
+        <v>38</v>
+      </c>
+      <c r="B17" s="14">
         <f>Data!E37</f>
         <v>8031.2257372654149</v>
       </c>

</xml_diff>